<commit_message>
Fix bug with cutoff point
</commit_message>
<xml_diff>
--- a/tests/testthat/Beispiel_Datenblatt_M1.xlsx
+++ b/tests/testthat/Beispiel_Datenblatt_M1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8876B9-467E-4E9D-BD6F-84BE6706A2CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4183D933-644D-4DA6-ACAB-8906C54667A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11303,12 +11303,6 @@
       <c r="F196" t="s">
         <v>49</v>
       </c>
-      <c r="G196">
-        <v>0</v>
-      </c>
-      <c r="H196">
-        <v>5</v>
-      </c>
       <c r="I196">
         <v>100</v>
       </c>
@@ -13158,12 +13152,6 @@
       <c r="F231" t="s">
         <v>49</v>
       </c>
-      <c r="G231">
-        <v>0</v>
-      </c>
-      <c r="H231">
-        <v>5</v>
-      </c>
       <c r="I231">
         <v>100</v>
       </c>
@@ -14483,12 +14471,6 @@
       <c r="F256" t="s">
         <v>49</v>
       </c>
-      <c r="G256">
-        <v>0</v>
-      </c>
-      <c r="H256">
-        <v>5</v>
-      </c>
       <c r="I256">
         <v>100</v>
       </c>
@@ -14536,12 +14518,6 @@
       <c r="F257" t="s">
         <v>49</v>
       </c>
-      <c r="G257">
-        <v>0</v>
-      </c>
-      <c r="H257">
-        <v>5</v>
-      </c>
       <c r="I257">
         <v>100</v>
       </c>
@@ -15966,12 +15942,6 @@
       </c>
       <c r="F284" t="s">
         <v>51</v>
-      </c>
-      <c r="G284">
-        <v>5</v>
-      </c>
-      <c r="H284">
-        <v>5</v>
       </c>
       <c r="I284">
         <v>100</v>

</xml_diff>